<commit_message>
adding some xls work from office PC
</commit_message>
<xml_diff>
--- a/AAHSL_memebers_data/AAHSL_members-JP.xlsx
+++ b/AAHSL_memebers_data/AAHSL_members-JP.xlsx
@@ -1,25 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
-  <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="17460" tabRatio="500"/>
+    <workbookView xWindow="120" yWindow="90" windowWidth="21075" windowHeight="8250"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="140000" concurrentCalc="0"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
-    </ext>
-  </extLst>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>instName</t>
   </si>
@@ -28,32 +25,25 @@
   </si>
   <si>
     <t>libUrl</t>
+  </si>
+  <si>
+    <t>Western University of Health Sciences</t>
+  </si>
+  <si>
+    <t>Harriet K. &amp; Philip Pumerantz Library</t>
+  </si>
+  <si>
+    <t>http://www.westernu.edu/library/</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
-      <sz val="12"/>
+      <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="12"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="12"/>
-      <color theme="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -76,25 +66,22 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="5">
-    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -243,16 +230,20 @@
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:tint val="100000"/>
-                <a:shade val="100000"/>
+                <a:shade val="51000"/>
                 <a:satMod val="130000"/>
               </a:schemeClr>
             </a:gs>
+            <a:gs pos="80000">
+              <a:schemeClr val="phClr">
+                <a:shade val="93000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:tint val="50000"/>
-                <a:shade val="100000"/>
-                <a:satMod val="350000"/>
+                <a:shade val="94000"/>
+                <a:satMod val="135000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
@@ -374,66 +365,27 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
-  <a:objectDefaults>
-    <a:spDef>
-      <a:spPr/>
-      <a:bodyPr/>
-      <a:lstStyle/>
-      <a:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="3">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="2">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </a:style>
-    </a:spDef>
-    <a:lnDef>
-      <a:spPr/>
-      <a:bodyPr/>
-      <a:lstStyle/>
-      <a:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </a:style>
-    </a:lnDef>
-  </a:objectDefaults>
+  <a:objectDefaults/>
   <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.33203125" customWidth="1"/>
-    <col min="2" max="2" width="25.33203125" customWidth="1"/>
-    <col min="3" max="3" width="24.83203125" customWidth="1"/>
+    <col min="1" max="1" width="35.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="34" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="32.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -444,13 +396,42 @@
         <v>2</v>
       </c>
     </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>